<commit_message>
sync tags adresses to mailjet
</commit_message>
<xml_diff>
--- a/public/files/import/test.xlsx
+++ b/public/files/import/test.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/shop/public/files/import/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4FE41B-963D-3444-A326-6FE77FE22A31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,16 +30,16 @@
     <t>cindy.leschaud@gmail.com</t>
   </si>
   <si>
-    <t>prunturt@yahoo.fr</t>
+    <t>email</t>
   </si>
   <si>
-    <t>email</t>
+    <t>pruntrut@yahoo.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,6 +98,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,31 +430,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>